<commit_message>
multiple sheets input feature
</commit_message>
<xml_diff>
--- a/app/ui_modules/input_file.xlsx
+++ b/app/ui_modules/input_file.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\python_web_reports_cient\app\ui_modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nagasudhir\python_web_reports_client\app\ui_modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
-    <sheet name="config" sheetId="2" r:id="rId2"/>
+    <sheet name="input_1" sheetId="4" r:id="rId2"/>
     <sheet name="all_keys" sheetId="3" r:id="rId3"/>
+    <sheet name="config" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">input!$A$1:$D$1490</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5967" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5985" uniqueCount="262">
   <si>
     <t>entity</t>
   </si>
@@ -1161,7 +1162,7 @@
   <dimension ref="A1:D1490"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22037,47 +22038,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>-10000</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>-10000</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>-10000</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>-10000</v>
+      </c>
+      <c r="D5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>-10000</v>
+      </c>
+      <c r="D6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>-10000</v>
+      </c>
+      <c r="D7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>-10000</v>
+      </c>
+      <c r="D8">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -34022,4 +34104,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ire keys in one sheet
</commit_message>
<xml_diff>
--- a/app/ui_modules/input_file.xlsx
+++ b/app/ui_modules/input_file.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
     <sheet name="input_1" sheetId="4" r:id="rId2"/>
-    <sheet name="all_keys" sheetId="3" r:id="rId3"/>
+    <sheet name="input_ire_mus" sheetId="5" r:id="rId3"/>
     <sheet name="config" sheetId="2" r:id="rId4"/>
+    <sheet name="all_keys" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">input!$A$1:$D$1490</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">input!$A$1:$D$1504</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6047" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6111" uniqueCount="264">
   <si>
     <t>entity</t>
   </si>
@@ -1167,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1504"/>
   <sheetViews>
-    <sheetView topLeftCell="A1490" workbookViewId="0">
-      <selection activeCell="D1501" sqref="D1501"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22234,6 +22235,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1504"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -22242,7 +22244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -22412,6 +22414,511 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>-10000</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>-10000</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>-10000</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>-10000</v>
+      </c>
+      <c r="D5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>-10000</v>
+      </c>
+      <c r="D6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>-10000</v>
+      </c>
+      <c r="D7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8">
+        <v>-10000</v>
+      </c>
+      <c r="D8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>-10000</v>
+      </c>
+      <c r="D9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>-10000</v>
+      </c>
+      <c r="D10">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>-10000</v>
+      </c>
+      <c r="D11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>-10000</v>
+      </c>
+      <c r="D12">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>-10000</v>
+      </c>
+      <c r="D13">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>-10000</v>
+      </c>
+      <c r="D14">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>-10000</v>
+      </c>
+      <c r="D15">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>-10000</v>
+      </c>
+      <c r="D16">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>-10000</v>
+      </c>
+      <c r="D17">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>-10000</v>
+      </c>
+      <c r="D18">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>-10000</v>
+      </c>
+      <c r="D19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>-10000</v>
+      </c>
+      <c r="D20">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>-10000</v>
+      </c>
+      <c r="D21">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>-10000</v>
+      </c>
+      <c r="D22">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>-10000</v>
+      </c>
+      <c r="D23">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>-10000</v>
+      </c>
+      <c r="D24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25" t="s">
+        <v>243</v>
+      </c>
+      <c r="C25">
+        <v>-10000</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>-10000</v>
+      </c>
+      <c r="D26">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>-10000</v>
+      </c>
+      <c r="D27">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>-10000</v>
+      </c>
+      <c r="D28">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>-10000</v>
+      </c>
+      <c r="D29">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>-10000</v>
+      </c>
+      <c r="D30">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31" t="s">
+        <v>243</v>
+      </c>
+      <c r="C31">
+        <v>-10000</v>
+      </c>
+      <c r="D31">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1504"/>
   <sheetViews>
@@ -34458,54 +34965,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>